<commit_message>
Commit with swahili_neg to the point where it should be :)
</commit_message>
<xml_diff>
--- a/Languages/swahili_excel.xlsx
+++ b/Languages/swahili_excel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alessio/Desktop/Projects/Language Independent Parser/Languages/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5541B87-8E36-7D42-92B6-ACE04793A97A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{685C0512-AF6A-3346-A765-987A8F78A16F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16360" xr2:uid="{BCE60CF4-7BA6-8843-A50E-A5C76864F2BB}"/>
   </bookViews>
@@ -283,10 +283,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -603,8 +602,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64028B3B-4BD0-9F48-9FE7-61D4119521D9}">
   <dimension ref="A1:E32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="158" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView tabSelected="1" zoomScale="158" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -644,7 +643,7 @@
       <c r="D2" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" t="s">
         <v>13</v>
       </c>
     </row>
@@ -814,7 +813,7 @@
       <c r="D12" t="s">
         <v>12</v>
       </c>
-      <c r="E12" s="2" t="s">
+      <c r="E12" t="s">
         <v>31</v>
       </c>
     </row>

</xml_diff>